<commit_message>
CRMS-902 MWH & OW Accessories Sales format Finalization
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/mwh_msl_data.xlsx
+++ b/application/controllers/excel-templates/mwh_msl_data.xlsx
@@ -20,7 +20,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
+  <si>
+    <t xml:space="preserve">Training Comments For Warehouse Sales Employees - For IW MWH Stock placement at SF pls consider Consumption and Recommendation Columns. For OW Stock Sale pls consider Number of Bookins landed (Repair &amp; DI) vs Sale of Parts in 4 months mentioned in columns towards last </t>
+  </si>
   <si>
     <t xml:space="preserve">Company Name</t>
   </si>
@@ -70,6 +73,27 @@
     <t xml:space="preserve">Recommended for 30 Days</t>
   </si>
   <si>
+    <t xml:space="preserve">RM Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ASM Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">State</t>
+  </si>
+  <si>
+    <t xml:space="preserve">City</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M-3 Month  Sale to SF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M-2Month  Sale to SF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">current-3 Month  Sale to SF</t>
+  </si>
+  <si>
     <t xml:space="preserve">{parts:company_name}</t>
   </si>
   <si>
@@ -116,6 +140,30 @@
   </si>
   <si>
     <t xml:space="preserve">{parts:recommended_30_days}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{parts:rm_name}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{parts:asm_name}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{parts:state}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{parts:district}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{parts:m3_sale_to_sf}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{parts:m2_sale_to_sf}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{parts:m1_sale_to_sf}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{parts:m_sale_to_sf}</t>
   </si>
 </sst>
 </file>
@@ -125,7 +173,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -149,6 +197,13 @@
       <family val="0"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Cambria"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <b val="true"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -157,19 +212,25 @@
       <charset val="1"/>
     </font>
     <font>
+      <b val="true"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Cambria"/>
-      <family val="0"/>
-      <charset val="1"/>
+      <family val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC4BD97"/>
+        <bgColor rgb="FFFFCC99"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -206,16 +267,28 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -228,6 +301,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC4BD97"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -236,76 +369,54 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AD1000"/>
+  <dimension ref="A1:AD1001"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I11" activeCellId="0" sqref="I11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="4" style="0" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="19.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="22.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="22.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="31.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="26.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="26.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="0" width="24.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="31.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="30.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="31.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="23.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="18" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="21.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="22.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="21.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="24.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="25" style="0" width="14.43"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
       <c r="R1" s="1"/>
       <c r="S1" s="1"/>
@@ -322,56 +433,159 @@
       <c r="AD1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="P2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="Q2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="R2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="S2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="T2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="U2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="V2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="W2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="X2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
+      <c r="AA2" s="3"/>
+      <c r="AB2" s="3"/>
+      <c r="AC2" s="3"/>
+      <c r="AD2" s="3"/>
+    </row>
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="B3" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="C3" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="D3" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="E3" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="F3" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="G3" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="H3" s="5" t="s">
         <v>31</v>
       </c>
+      <c r="I3" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="N3" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="O3" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="P3" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q3" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="R3" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="S3" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="T3" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="U3" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="V3" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="W3" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="X3" s="5" t="s">
+        <v>47</v>
+      </c>
     </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1369,7 +1583,11 @@
     <row r="998" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="999" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1000" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1001" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:X1"/>
+  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>